<commit_message>
ADD verification to labels
</commit_message>
<xml_diff>
--- a/test_images/apples_images/apples_images_mroi/mroi_labeled_features.xlsx
+++ b/test_images/apples_images/apples_images_mroi/mroi_labeled_features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauro\Desktop\Riccardo Carroccio\CV@TR2\test_images\apples_images\apples_images_mroi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC3E54C-6768-402B-8FD2-7FA76D476009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B2FB99-025B-419F-A8D9-E0A6F993A365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3546,7 +3546,7 @@
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C40">
@@ -3617,7 +3617,7 @@
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C41">
@@ -3688,7 +3688,7 @@
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C42">
@@ -3759,7 +3759,7 @@
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C43">
@@ -3830,7 +3830,7 @@
       <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C44">
@@ -3901,7 +3901,7 @@
       <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C45">
@@ -3972,7 +3972,7 @@
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C46">
@@ -4043,7 +4043,7 @@
       <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C47">
@@ -4114,7 +4114,7 @@
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C48">
@@ -4185,7 +4185,7 @@
       <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C49">
@@ -4327,7 +4327,7 @@
       <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C51">
@@ -4398,7 +4398,7 @@
       <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C52">
@@ -4469,7 +4469,7 @@
       <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C53">
@@ -4540,7 +4540,7 @@
       <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C54">
@@ -4611,7 +4611,7 @@
       <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C55">
@@ -4682,7 +4682,7 @@
       <c r="A56" t="s">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C56">
@@ -4753,7 +4753,7 @@
       <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C57">
@@ -4824,7 +4824,7 @@
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C58">
@@ -4895,7 +4895,7 @@
       <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C59">
@@ -4966,7 +4966,7 @@
       <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C60">
@@ -5037,7 +5037,7 @@
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C61">
@@ -5108,7 +5108,7 @@
       <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C62">
@@ -5179,7 +5179,7 @@
       <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C63">
@@ -5250,7 +5250,7 @@
       <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C64">
@@ -5321,7 +5321,7 @@
       <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C65">
@@ -5392,7 +5392,7 @@
       <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C66">
@@ -5463,7 +5463,7 @@
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C67">
@@ -5605,7 +5605,7 @@
       <c r="A69" t="s">
         <v>68</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C69">
@@ -5676,7 +5676,7 @@
       <c r="A70" t="s">
         <v>69</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C70">

</xml_diff>